<commit_message>
Two-nodes and fix one
</commit_message>
<xml_diff>
--- a/mdone_one_node.xlsx
+++ b/mdone_one_node.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I158"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,13 +484,13 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.00015</v>
+        <v>0.00557</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00015</v>
+        <v>0.00557</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00015</v>
+        <v>0.00557</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -511,13 +511,13 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00015</v>
+        <v>0.00557</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00015</v>
+        <v>0.00557</v>
       </c>
       <c r="E4" t="n">
-        <v>0.00016</v>
+        <v>0.00558</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -538,7 +538,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00016</v>
+        <v>0.00558</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
@@ -567,13 +567,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0.00054</v>
+        <v>0.00781</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00054</v>
+        <v>0.00781</v>
       </c>
       <c r="E6" t="n">
-        <v>0.00054</v>
+        <v>0.00781</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -594,13 +594,13 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>0.00054</v>
+        <v>0.00781</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00054</v>
+        <v>0.00781</v>
       </c>
       <c r="E7" t="n">
-        <v>0.00055</v>
+        <v>0.00783</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -621,7 +621,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="n">
-        <v>0.00055</v>
+        <v>0.00783</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
@@ -650,13 +650,13 @@
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00059</v>
+        <v>0.0089</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00059</v>
+        <v>0.0089</v>
       </c>
       <c r="E9" t="n">
-        <v>0.00059</v>
+        <v>0.0089</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -677,13 +677,13 @@
         <v>2</v>
       </c>
       <c r="C10" t="n">
-        <v>0.00059</v>
+        <v>0.0089</v>
       </c>
       <c r="D10" t="n">
-        <v>0.00059</v>
+        <v>0.0089</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00891</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -704,7 +704,7 @@
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0005999999999999999</v>
+        <v>0.00891</v>
       </c>
       <c r="D11" t="n">
         <v>0</v>
@@ -722,7 +722,7 @@
         <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>1e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="12">
@@ -733,13 +733,13 @@
         <v>3</v>
       </c>
       <c r="C12" t="n">
-        <v>0.00073</v>
+        <v>0.01327</v>
       </c>
       <c r="D12" t="n">
-        <v>0.00073</v>
+        <v>0.01327</v>
       </c>
       <c r="E12" t="n">
-        <v>0.00076</v>
+        <v>0.01327</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -760,13 +760,13 @@
         <v>3</v>
       </c>
       <c r="C13" t="n">
-        <v>0.00076</v>
+        <v>0.01327</v>
       </c>
       <c r="D13" t="n">
-        <v>0.00076</v>
+        <v>0.01327</v>
       </c>
       <c r="E13" t="n">
-        <v>0.00077</v>
+        <v>0.01328</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -787,7 +787,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00077</v>
+        <v>0.01328</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
@@ -805,7 +805,7 @@
         <v>3</v>
       </c>
       <c r="I14" t="n">
-        <v>3e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="15">
@@ -816,13 +816,13 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>0.01358</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>0.01358</v>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>0.01358</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -831,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="inlineStr"/>
     </row>
@@ -843,13 +843,13 @@
         <v>4</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>0.01358</v>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>0.01358</v>
       </c>
       <c r="E16" t="n">
-        <v>1e-05</v>
+        <v>0.01359</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -870,7 +870,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="n">
-        <v>1e-05</v>
+        <v>0.01359</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
@@ -899,13 +899,13 @@
         <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>2e-05</v>
+        <v>0.02136</v>
       </c>
       <c r="D18" t="n">
-        <v>2e-05</v>
+        <v>0.02136</v>
       </c>
       <c r="E18" t="n">
-        <v>2e-05</v>
+        <v>0.02136</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -914,7 +914,7 @@
         <v>1</v>
       </c>
       <c r="H18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" t="inlineStr"/>
     </row>
@@ -926,13 +926,13 @@
         <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>2e-05</v>
+        <v>0.02136</v>
       </c>
       <c r="D19" t="n">
-        <v>2e-05</v>
+        <v>0.02136</v>
       </c>
       <c r="E19" t="n">
-        <v>3e-05</v>
+        <v>0.02138</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -953,7 +953,7 @@
         <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>3e-05</v>
+        <v>0.02138</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -982,13 +982,13 @@
         <v>6</v>
       </c>
       <c r="C21" t="n">
-        <v>3e-05</v>
+        <v>0.02474</v>
       </c>
       <c r="D21" t="n">
-        <v>3e-05</v>
+        <v>0.02474</v>
       </c>
       <c r="E21" t="n">
-        <v>3e-05</v>
+        <v>0.02474</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="H21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I21" t="inlineStr"/>
     </row>
@@ -1009,13 +1009,13 @@
         <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>3e-05</v>
+        <v>0.02474</v>
       </c>
       <c r="D22" t="n">
-        <v>3e-05</v>
+        <v>0.02474</v>
       </c>
       <c r="E22" t="n">
-        <v>5e-05</v>
+        <v>0.02476</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -1036,7 +1036,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>5e-05</v>
+        <v>0.02476</v>
       </c>
       <c r="D23" t="n">
         <v>0</v>
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="I23" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="24">
@@ -1065,13 +1065,13 @@
         <v>7</v>
       </c>
       <c r="C24" t="n">
-        <v>4e-05</v>
+        <v>0.02685</v>
       </c>
       <c r="D24" t="n">
-        <v>4e-05</v>
+        <v>0.02685</v>
       </c>
       <c r="E24" t="n">
-        <v>5e-05</v>
+        <v>0.02685</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1080,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="H24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="inlineStr"/>
     </row>
@@ -1092,13 +1092,13 @@
         <v>7</v>
       </c>
       <c r="C25" t="n">
-        <v>5e-05</v>
+        <v>0.02685</v>
       </c>
       <c r="D25" t="n">
-        <v>5e-05</v>
+        <v>0.02685</v>
       </c>
       <c r="E25" t="n">
-        <v>6e-05</v>
+        <v>0.02687</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1119,7 +1119,7 @@
         <v>7</v>
       </c>
       <c r="C26" t="n">
-        <v>6e-05</v>
+        <v>0.02687</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
@@ -1148,22 +1148,22 @@
         <v>8</v>
       </c>
       <c r="C27" t="n">
-        <v>4e-05</v>
+        <v>0.03368</v>
       </c>
       <c r="D27" t="n">
-        <v>5e-05</v>
+        <v>0.03368</v>
       </c>
       <c r="E27" t="n">
-        <v>6e-05</v>
+        <v>0.03368</v>
       </c>
       <c r="F27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="inlineStr"/>
     </row>
@@ -1175,13 +1175,13 @@
         <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>6e-05</v>
+        <v>0.03368</v>
       </c>
       <c r="D28" t="n">
-        <v>6e-05</v>
+        <v>0.03368</v>
       </c>
       <c r="E28" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0.03369</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1202,7 +1202,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="n">
-        <v>6.999999999999999e-05</v>
+        <v>0.03369</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
@@ -1220,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="I29" t="n">
-        <v>3e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="30">
@@ -1231,13 +1231,13 @@
         <v>9</v>
       </c>
       <c r="C30" t="n">
-        <v>0.00011</v>
+        <v>0.03661</v>
       </c>
       <c r="D30" t="n">
-        <v>0.00011</v>
+        <v>0.03661</v>
       </c>
       <c r="E30" t="n">
-        <v>0.00011</v>
+        <v>0.03662</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1246,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30" t="inlineStr"/>
     </row>
@@ -1258,13 +1258,13 @@
         <v>9</v>
       </c>
       <c r="C31" t="n">
-        <v>0.00011</v>
+        <v>0.03662</v>
       </c>
       <c r="D31" t="n">
-        <v>0.00011</v>
+        <v>0.03662</v>
       </c>
       <c r="E31" t="n">
-        <v>0.00012</v>
+        <v>0.03663</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1285,7 +1285,7 @@
         <v>9</v>
       </c>
       <c r="C32" t="n">
-        <v>0.00012</v>
+        <v>0.03663</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
@@ -1303,7 +1303,7 @@
         <v>3</v>
       </c>
       <c r="I32" t="n">
-        <v>1e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="33">
@@ -1314,13 +1314,13 @@
         <v>10</v>
       </c>
       <c r="C33" t="n">
-        <v>0.00015</v>
+        <v>0.03687</v>
       </c>
       <c r="D33" t="n">
-        <v>0.00015</v>
+        <v>0.03687</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00016</v>
+        <v>0.03687</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1329,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="H33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33" t="inlineStr"/>
     </row>
@@ -1341,13 +1341,13 @@
         <v>10</v>
       </c>
       <c r="C34" t="n">
-        <v>0.00016</v>
+        <v>0.03687</v>
       </c>
       <c r="D34" t="n">
-        <v>0.00016</v>
+        <v>0.03687</v>
       </c>
       <c r="E34" t="n">
-        <v>0.00017</v>
+        <v>0.03689</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1368,7 +1368,7 @@
         <v>10</v>
       </c>
       <c r="C35" t="n">
-        <v>0.00017</v>
+        <v>0.03689</v>
       </c>
       <c r="D35" t="n">
         <v>0</v>
@@ -1386,7 +1386,7 @@
         <v>3</v>
       </c>
       <c r="I35" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="36">
@@ -1397,22 +1397,22 @@
         <v>11</v>
       </c>
       <c r="C36" t="n">
-        <v>0.00015</v>
+        <v>0.04101</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00016</v>
+        <v>0.04101</v>
       </c>
       <c r="E36" t="n">
-        <v>0.00017</v>
+        <v>0.04101</v>
       </c>
       <c r="F36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G36" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" t="inlineStr"/>
     </row>
@@ -1424,13 +1424,13 @@
         <v>11</v>
       </c>
       <c r="C37" t="n">
-        <v>0.00017</v>
+        <v>0.04101</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00017</v>
+        <v>0.04101</v>
       </c>
       <c r="E37" t="n">
-        <v>0.00018</v>
+        <v>0.04102</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1451,7 +1451,7 @@
         <v>11</v>
       </c>
       <c r="C38" t="n">
-        <v>0.00018</v>
+        <v>0.04102</v>
       </c>
       <c r="D38" t="n">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>3</v>
       </c>
       <c r="I38" t="n">
-        <v>3e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="39">
@@ -1480,22 +1480,22 @@
         <v>12</v>
       </c>
       <c r="C39" t="n">
-        <v>0.00017</v>
+        <v>0.0425</v>
       </c>
       <c r="D39" t="n">
-        <v>0.00017</v>
+        <v>0.0425</v>
       </c>
       <c r="E39" t="n">
-        <v>0.00018</v>
+        <v>0.04251</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" t="inlineStr"/>
     </row>
@@ -1507,13 +1507,13 @@
         <v>12</v>
       </c>
       <c r="C40" t="n">
-        <v>0.00018</v>
+        <v>0.04251</v>
       </c>
       <c r="D40" t="n">
-        <v>0.00018</v>
+        <v>0.04251</v>
       </c>
       <c r="E40" t="n">
-        <v>0.00019</v>
+        <v>0.04252</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1534,7 +1534,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="n">
-        <v>0.00019</v>
+        <v>0.04252</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -1552,7 +1552,7 @@
         <v>3</v>
       </c>
       <c r="I41" t="n">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="42">
@@ -1563,13 +1563,13 @@
         <v>13</v>
       </c>
       <c r="C42" t="n">
-        <v>0.00019</v>
+        <v>0.07063999999999999</v>
       </c>
       <c r="D42" t="n">
-        <v>0.00019</v>
+        <v>0.07063999999999999</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00019</v>
+        <v>0.07063999999999999</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1578,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="inlineStr"/>
     </row>
@@ -1590,13 +1590,13 @@
         <v>13</v>
       </c>
       <c r="C43" t="n">
-        <v>0.00019</v>
+        <v>0.07063999999999999</v>
       </c>
       <c r="D43" t="n">
-        <v>0.00019</v>
+        <v>0.07063999999999999</v>
       </c>
       <c r="E43" t="n">
-        <v>0.00021</v>
+        <v>0.07066</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1617,7 +1617,7 @@
         <v>13</v>
       </c>
       <c r="C44" t="n">
-        <v>0.00021</v>
+        <v>0.07066</v>
       </c>
       <c r="D44" t="n">
         <v>0</v>
@@ -1635,7 +1635,7 @@
         <v>3</v>
       </c>
       <c r="I44" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="45">
@@ -1646,13 +1646,13 @@
         <v>14</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0002</v>
+        <v>0.07188</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0002</v>
+        <v>0.07188</v>
       </c>
       <c r="E45" t="n">
-        <v>0.00021</v>
+        <v>0.07188</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1661,7 +1661,7 @@
         <v>1</v>
       </c>
       <c r="H45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" t="inlineStr"/>
     </row>
@@ -1673,13 +1673,13 @@
         <v>14</v>
       </c>
       <c r="C46" t="n">
-        <v>0.00021</v>
+        <v>0.07188</v>
       </c>
       <c r="D46" t="n">
-        <v>0.00021</v>
+        <v>0.07188</v>
       </c>
       <c r="E46" t="n">
-        <v>0.00022</v>
+        <v>0.07189</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1700,7 +1700,7 @@
         <v>14</v>
       </c>
       <c r="C47" t="n">
-        <v>0.00022</v>
+        <v>0.07189</v>
       </c>
       <c r="D47" t="n">
         <v>0</v>
@@ -1718,7 +1718,7 @@
         <v>3</v>
       </c>
       <c r="I47" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="48">
@@ -1729,13 +1729,13 @@
         <v>15</v>
       </c>
       <c r="C48" t="n">
-        <v>0.00021</v>
+        <v>0.07696</v>
       </c>
       <c r="D48" t="n">
-        <v>0.00021</v>
+        <v>0.07696</v>
       </c>
       <c r="E48" t="n">
-        <v>0.00022</v>
+        <v>0.07697</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1744,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="H48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" t="inlineStr"/>
     </row>
@@ -1756,13 +1756,13 @@
         <v>15</v>
       </c>
       <c r="C49" t="n">
-        <v>0.00022</v>
+        <v>0.07697</v>
       </c>
       <c r="D49" t="n">
-        <v>0.00022</v>
+        <v>0.07697</v>
       </c>
       <c r="E49" t="n">
-        <v>0.00023</v>
+        <v>0.07698000000000001</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1783,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="C50" t="n">
-        <v>0.00023</v>
+        <v>0.07698000000000001</v>
       </c>
       <c r="D50" t="n">
         <v>0</v>
@@ -1812,13 +1812,13 @@
         <v>16</v>
       </c>
       <c r="C51" t="n">
-        <v>0.00024</v>
+        <v>0.08161</v>
       </c>
       <c r="D51" t="n">
-        <v>0.00024</v>
+        <v>0.08161</v>
       </c>
       <c r="E51" t="n">
-        <v>0.00024</v>
+        <v>0.08161</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
@@ -1827,7 +1827,7 @@
         <v>1</v>
       </c>
       <c r="H51" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" t="inlineStr"/>
     </row>
@@ -1839,13 +1839,13 @@
         <v>16</v>
       </c>
       <c r="C52" t="n">
-        <v>0.00024</v>
+        <v>0.08161</v>
       </c>
       <c r="D52" t="n">
-        <v>0.00024</v>
+        <v>0.08161</v>
       </c>
       <c r="E52" t="n">
-        <v>0.00025</v>
+        <v>0.08162</v>
       </c>
       <c r="F52" t="n">
         <v>0</v>
@@ -1866,7 +1866,7 @@
         <v>16</v>
       </c>
       <c r="C53" t="n">
-        <v>0.00025</v>
+        <v>0.08162</v>
       </c>
       <c r="D53" t="n">
         <v>0</v>
@@ -1895,13 +1895,13 @@
         <v>17</v>
       </c>
       <c r="C54" t="n">
-        <v>0.00024</v>
+        <v>0.0843</v>
       </c>
       <c r="D54" t="n">
-        <v>0.00024</v>
+        <v>0.0843</v>
       </c>
       <c r="E54" t="n">
-        <v>0.00025</v>
+        <v>0.0843</v>
       </c>
       <c r="F54" t="n">
         <v>0</v>
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" t="inlineStr"/>
     </row>
@@ -1922,13 +1922,13 @@
         <v>17</v>
       </c>
       <c r="C55" t="n">
-        <v>0.00025</v>
+        <v>0.0843</v>
       </c>
       <c r="D55" t="n">
-        <v>0.00025</v>
+        <v>0.0843</v>
       </c>
       <c r="E55" t="n">
-        <v>0.00026</v>
+        <v>0.08431</v>
       </c>
       <c r="F55" t="n">
         <v>0</v>
@@ -1949,7 +1949,7 @@
         <v>17</v>
       </c>
       <c r="C56" t="n">
-        <v>0.00026</v>
+        <v>0.08431</v>
       </c>
       <c r="D56" t="n">
         <v>0</v>
@@ -1967,7 +1967,7 @@
         <v>3</v>
       </c>
       <c r="I56" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="57">
@@ -1978,13 +1978,13 @@
         <v>18</v>
       </c>
       <c r="C57" t="n">
-        <v>0.00026</v>
+        <v>0.08723</v>
       </c>
       <c r="D57" t="n">
-        <v>0.00026</v>
+        <v>0.08723</v>
       </c>
       <c r="E57" t="n">
-        <v>0.00026</v>
+        <v>0.08723</v>
       </c>
       <c r="F57" t="n">
         <v>0</v>
@@ -1993,7 +1993,7 @@
         <v>1</v>
       </c>
       <c r="H57" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" t="inlineStr"/>
     </row>
@@ -2005,13 +2005,13 @@
         <v>18</v>
       </c>
       <c r="C58" t="n">
-        <v>0.00026</v>
+        <v>0.08723</v>
       </c>
       <c r="D58" t="n">
-        <v>0.00026</v>
+        <v>0.08723</v>
       </c>
       <c r="E58" t="n">
-        <v>0.00028</v>
+        <v>0.08724999999999999</v>
       </c>
       <c r="F58" t="n">
         <v>0</v>
@@ -2032,7 +2032,7 @@
         <v>18</v>
       </c>
       <c r="C59" t="n">
-        <v>0.00028</v>
+        <v>0.08724999999999999</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
@@ -2061,13 +2061,13 @@
         <v>19</v>
       </c>
       <c r="C60" t="n">
-        <v>0.00027</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="D60" t="n">
-        <v>0.00027</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="E60" t="n">
-        <v>0.00028</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="F60" t="n">
         <v>0</v>
@@ -2076,7 +2076,7 @@
         <v>1</v>
       </c>
       <c r="H60" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" t="inlineStr"/>
     </row>
@@ -2088,13 +2088,13 @@
         <v>19</v>
       </c>
       <c r="C61" t="n">
-        <v>0.00028</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="D61" t="n">
-        <v>0.00028</v>
+        <v>0.08939999999999999</v>
       </c>
       <c r="E61" t="n">
-        <v>0.00029</v>
+        <v>0.08942</v>
       </c>
       <c r="F61" t="n">
         <v>0</v>
@@ -2115,7 +2115,7 @@
         <v>19</v>
       </c>
       <c r="C62" t="n">
-        <v>0.00029</v>
+        <v>0.08942</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
@@ -2133,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="I62" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="63">
@@ -2144,13 +2144,13 @@
         <v>20</v>
       </c>
       <c r="C63" t="n">
-        <v>0.00028</v>
+        <v>0.09671</v>
       </c>
       <c r="D63" t="n">
-        <v>0.00028</v>
+        <v>0.09671</v>
       </c>
       <c r="E63" t="n">
-        <v>0.00029</v>
+        <v>0.09672</v>
       </c>
       <c r="F63" t="n">
         <v>0</v>
@@ -2159,7 +2159,7 @@
         <v>1</v>
       </c>
       <c r="H63" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" t="inlineStr"/>
     </row>
@@ -2171,13 +2171,13 @@
         <v>20</v>
       </c>
       <c r="C64" t="n">
-        <v>0.00029</v>
+        <v>0.09672</v>
       </c>
       <c r="D64" t="n">
-        <v>0.00029</v>
+        <v>0.09672</v>
       </c>
       <c r="E64" t="n">
-        <v>0.0003</v>
+        <v>0.09674000000000001</v>
       </c>
       <c r="F64" t="n">
         <v>0</v>
@@ -2198,7 +2198,7 @@
         <v>20</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0003</v>
+        <v>0.09674000000000001</v>
       </c>
       <c r="D65" t="n">
         <v>0</v>
@@ -2227,13 +2227,13 @@
         <v>21</v>
       </c>
       <c r="C66" t="n">
-        <v>0.00031</v>
+        <v>0.10177</v>
       </c>
       <c r="D66" t="n">
-        <v>0.00031</v>
+        <v>0.10177</v>
       </c>
       <c r="E66" t="n">
-        <v>0.00031</v>
+        <v>0.10178</v>
       </c>
       <c r="F66" t="n">
         <v>0</v>
@@ -2242,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="H66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" t="inlineStr"/>
     </row>
@@ -2254,13 +2254,13 @@
         <v>21</v>
       </c>
       <c r="C67" t="n">
-        <v>0.00031</v>
+        <v>0.10178</v>
       </c>
       <c r="D67" t="n">
-        <v>0.00031</v>
+        <v>0.10178</v>
       </c>
       <c r="E67" t="n">
-        <v>0.00032</v>
+        <v>0.10179</v>
       </c>
       <c r="F67" t="n">
         <v>0</v>
@@ -2281,7 +2281,7 @@
         <v>21</v>
       </c>
       <c r="C68" t="n">
-        <v>0.00032</v>
+        <v>0.10179</v>
       </c>
       <c r="D68" t="n">
         <v>0</v>
@@ -2310,13 +2310,13 @@
         <v>22</v>
       </c>
       <c r="C69" t="n">
-        <v>0.00031</v>
+        <v>0.10731</v>
       </c>
       <c r="D69" t="n">
-        <v>0.00031</v>
+        <v>0.10731</v>
       </c>
       <c r="E69" t="n">
-        <v>0.00032</v>
+        <v>0.10731</v>
       </c>
       <c r="F69" t="n">
         <v>0</v>
@@ -2325,7 +2325,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" t="inlineStr"/>
     </row>
@@ -2337,13 +2337,13 @@
         <v>22</v>
       </c>
       <c r="C70" t="n">
-        <v>0.00032</v>
+        <v>0.10731</v>
       </c>
       <c r="D70" t="n">
-        <v>0.00032</v>
+        <v>0.10731</v>
       </c>
       <c r="E70" t="n">
-        <v>0.00033</v>
+        <v>0.10732</v>
       </c>
       <c r="F70" t="n">
         <v>0</v>
@@ -2364,7 +2364,7 @@
         <v>22</v>
       </c>
       <c r="C71" t="n">
-        <v>0.00033</v>
+        <v>0.10732</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -2382,7 +2382,7 @@
         <v>3</v>
       </c>
       <c r="I71" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="72">
@@ -2393,13 +2393,13 @@
         <v>23</v>
       </c>
       <c r="C72" t="n">
-        <v>0.00032</v>
+        <v>0.11428</v>
       </c>
       <c r="D72" t="n">
-        <v>0.00032</v>
+        <v>0.11428</v>
       </c>
       <c r="E72" t="n">
-        <v>0.00033</v>
+        <v>0.11428</v>
       </c>
       <c r="F72" t="n">
         <v>0</v>
@@ -2408,7 +2408,7 @@
         <v>1</v>
       </c>
       <c r="H72" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" t="inlineStr"/>
     </row>
@@ -2420,13 +2420,13 @@
         <v>23</v>
       </c>
       <c r="C73" t="n">
-        <v>0.00033</v>
+        <v>0.11428</v>
       </c>
       <c r="D73" t="n">
-        <v>0.00033</v>
+        <v>0.11428</v>
       </c>
       <c r="E73" t="n">
-        <v>0.00035</v>
+        <v>0.1143</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -2447,7 +2447,7 @@
         <v>23</v>
       </c>
       <c r="C74" t="n">
-        <v>0.00035</v>
+        <v>0.1143</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
@@ -2465,7 +2465,7 @@
         <v>3</v>
       </c>
       <c r="I74" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="75">
@@ -2476,13 +2476,13 @@
         <v>24</v>
       </c>
       <c r="C75" t="n">
-        <v>0.00038</v>
+        <v>0.11648</v>
       </c>
       <c r="D75" t="n">
-        <v>0.00038</v>
+        <v>0.11648</v>
       </c>
       <c r="E75" t="n">
-        <v>0.00038</v>
+        <v>0.11648</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -2491,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="H75" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I75" t="inlineStr"/>
     </row>
@@ -2503,13 +2503,13 @@
         <v>24</v>
       </c>
       <c r="C76" t="n">
-        <v>0.00038</v>
+        <v>0.11648</v>
       </c>
       <c r="D76" t="n">
-        <v>0.00038</v>
+        <v>0.11648</v>
       </c>
       <c r="E76" t="n">
-        <v>0.0004</v>
+        <v>0.1165</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -2530,7 +2530,7 @@
         <v>24</v>
       </c>
       <c r="C77" t="n">
-        <v>0.0004</v>
+        <v>0.1165</v>
       </c>
       <c r="D77" t="n">
         <v>0</v>
@@ -2548,7 +2548,7 @@
         <v>3</v>
       </c>
       <c r="I77" t="n">
-        <v>1e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="78">
@@ -2559,13 +2559,13 @@
         <v>25</v>
       </c>
       <c r="C78" t="n">
-        <v>0.00039</v>
+        <v>0.11949</v>
       </c>
       <c r="D78" t="n">
-        <v>0.00039</v>
+        <v>0.11949</v>
       </c>
       <c r="E78" t="n">
-        <v>0.0004</v>
+        <v>0.11952</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -2574,7 +2574,7 @@
         <v>1</v>
       </c>
       <c r="H78" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I78" t="inlineStr"/>
     </row>
@@ -2586,13 +2586,13 @@
         <v>25</v>
       </c>
       <c r="C79" t="n">
-        <v>0.0004</v>
+        <v>0.11952</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0004</v>
+        <v>0.11952</v>
       </c>
       <c r="E79" t="n">
-        <v>0.00041</v>
+        <v>0.11953</v>
       </c>
       <c r="F79" t="n">
         <v>0</v>
@@ -2613,7 +2613,7 @@
         <v>25</v>
       </c>
       <c r="C80" t="n">
-        <v>0.00041</v>
+        <v>0.11953</v>
       </c>
       <c r="D80" t="n">
         <v>0</v>
@@ -2631,7 +2631,7 @@
         <v>3</v>
       </c>
       <c r="I80" t="n">
-        <v>2e-05</v>
+        <v>4e-05</v>
       </c>
     </row>
     <row r="81">
@@ -2642,13 +2642,13 @@
         <v>26</v>
       </c>
       <c r="C81" t="n">
-        <v>0.0004</v>
+        <v>0.12465</v>
       </c>
       <c r="D81" t="n">
-        <v>0.0004</v>
+        <v>0.12465</v>
       </c>
       <c r="E81" t="n">
-        <v>0.00041</v>
+        <v>0.12465</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -2657,7 +2657,7 @@
         <v>1</v>
       </c>
       <c r="H81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I81" t="inlineStr"/>
     </row>
@@ -2669,13 +2669,13 @@
         <v>26</v>
       </c>
       <c r="C82" t="n">
-        <v>0.00041</v>
+        <v>0.12465</v>
       </c>
       <c r="D82" t="n">
-        <v>0.00041</v>
+        <v>0.12465</v>
       </c>
       <c r="E82" t="n">
-        <v>0.00042</v>
+        <v>0.12467</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -2696,7 +2696,7 @@
         <v>26</v>
       </c>
       <c r="C83" t="n">
-        <v>0.00042</v>
+        <v>0.12467</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
@@ -2714,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="I83" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="84">
@@ -2725,13 +2725,13 @@
         <v>27</v>
       </c>
       <c r="C84" t="n">
-        <v>0.00042</v>
+        <v>0.12674</v>
       </c>
       <c r="D84" t="n">
-        <v>0.00042</v>
+        <v>0.12674</v>
       </c>
       <c r="E84" t="n">
-        <v>0.00042</v>
+        <v>0.12674</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -2740,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="H84" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="inlineStr"/>
     </row>
@@ -2752,13 +2752,13 @@
         <v>27</v>
       </c>
       <c r="C85" t="n">
-        <v>0.00042</v>
+        <v>0.12674</v>
       </c>
       <c r="D85" t="n">
-        <v>0.00042</v>
+        <v>0.12674</v>
       </c>
       <c r="E85" t="n">
-        <v>0.00043</v>
+        <v>0.12675</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -2779,7 +2779,7 @@
         <v>27</v>
       </c>
       <c r="C86" t="n">
-        <v>0.00043</v>
+        <v>0.12675</v>
       </c>
       <c r="D86" t="n">
         <v>0</v>
@@ -2808,13 +2808,13 @@
         <v>28</v>
       </c>
       <c r="C87" t="n">
-        <v>0.00042</v>
+        <v>0.12996</v>
       </c>
       <c r="D87" t="n">
-        <v>0.00042</v>
+        <v>0.12996</v>
       </c>
       <c r="E87" t="n">
-        <v>0.00043</v>
+        <v>0.12996</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -2823,7 +2823,7 @@
         <v>1</v>
       </c>
       <c r="H87" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I87" t="inlineStr"/>
     </row>
@@ -2835,13 +2835,13 @@
         <v>28</v>
       </c>
       <c r="C88" t="n">
-        <v>0.00043</v>
+        <v>0.12996</v>
       </c>
       <c r="D88" t="n">
-        <v>0.00043</v>
+        <v>0.12996</v>
       </c>
       <c r="E88" t="n">
-        <v>0.00045</v>
+        <v>0.12997</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -2862,7 +2862,7 @@
         <v>28</v>
       </c>
       <c r="C89" t="n">
-        <v>0.00045</v>
+        <v>0.12997</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
@@ -2880,7 +2880,7 @@
         <v>3</v>
       </c>
       <c r="I89" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="90">
@@ -2891,13 +2891,13 @@
         <v>29</v>
       </c>
       <c r="C90" t="n">
-        <v>0.00045</v>
+        <v>0.13032</v>
       </c>
       <c r="D90" t="n">
-        <v>0.00045</v>
+        <v>0.13032</v>
       </c>
       <c r="E90" t="n">
-        <v>0.00045</v>
+        <v>0.13032</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -2906,7 +2906,7 @@
         <v>1</v>
       </c>
       <c r="H90" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90" t="inlineStr"/>
     </row>
@@ -2918,13 +2918,13 @@
         <v>29</v>
       </c>
       <c r="C91" t="n">
-        <v>0.00045</v>
+        <v>0.13032</v>
       </c>
       <c r="D91" t="n">
-        <v>0.00045</v>
+        <v>0.13032</v>
       </c>
       <c r="E91" t="n">
-        <v>0.00046</v>
+        <v>0.13033</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -2945,7 +2945,7 @@
         <v>29</v>
       </c>
       <c r="C92" t="n">
-        <v>0.00046</v>
+        <v>0.13033</v>
       </c>
       <c r="D92" t="n">
         <v>0</v>
@@ -2974,13 +2974,13 @@
         <v>30</v>
       </c>
       <c r="C93" t="n">
-        <v>0.00045</v>
+        <v>0.13103</v>
       </c>
       <c r="D93" t="n">
-        <v>0.00045</v>
+        <v>0.13103</v>
       </c>
       <c r="E93" t="n">
-        <v>0.00046</v>
+        <v>0.13103</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -2989,7 +2989,7 @@
         <v>1</v>
       </c>
       <c r="H93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I93" t="inlineStr"/>
     </row>
@@ -3001,13 +3001,13 @@
         <v>30</v>
       </c>
       <c r="C94" t="n">
-        <v>0.00046</v>
+        <v>0.13103</v>
       </c>
       <c r="D94" t="n">
-        <v>0.00046</v>
+        <v>0.13103</v>
       </c>
       <c r="E94" t="n">
-        <v>0.00048</v>
+        <v>0.13105</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -3028,7 +3028,7 @@
         <v>30</v>
       </c>
       <c r="C95" t="n">
-        <v>0.00048</v>
+        <v>0.13105</v>
       </c>
       <c r="D95" t="n">
         <v>0</v>
@@ -3046,7 +3046,7 @@
         <v>3</v>
       </c>
       <c r="I95" t="n">
-        <v>2e-05</v>
+        <v>1e-05</v>
       </c>
     </row>
     <row r="96">
@@ -3057,22 +3057,22 @@
         <v>31</v>
       </c>
       <c r="C96" t="n">
-        <v>0.00045</v>
+        <v>0.1313</v>
       </c>
       <c r="D96" t="n">
-        <v>0.00046</v>
+        <v>0.1313</v>
       </c>
       <c r="E96" t="n">
-        <v>0.00048</v>
+        <v>0.13131</v>
       </c>
       <c r="F96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G96" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I96" t="inlineStr"/>
     </row>
@@ -3084,13 +3084,13 @@
         <v>31</v>
       </c>
       <c r="C97" t="n">
-        <v>0.00048</v>
+        <v>0.13131</v>
       </c>
       <c r="D97" t="n">
-        <v>0.00048</v>
+        <v>0.13131</v>
       </c>
       <c r="E97" t="n">
-        <v>0.00049</v>
+        <v>0.13132</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -3111,7 +3111,7 @@
         <v>31</v>
       </c>
       <c r="C98" t="n">
-        <v>0.00049</v>
+        <v>0.13132</v>
       </c>
       <c r="D98" t="n">
         <v>0</v>
@@ -3129,7 +3129,7 @@
         <v>3</v>
       </c>
       <c r="I98" t="n">
-        <v>3e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="99">
@@ -3140,22 +3140,22 @@
         <v>32</v>
       </c>
       <c r="C99" t="n">
-        <v>0.00045</v>
+        <v>0.13284</v>
       </c>
       <c r="D99" t="n">
-        <v>0.00048</v>
+        <v>0.13284</v>
       </c>
       <c r="E99" t="n">
-        <v>0.00049</v>
+        <v>0.13285</v>
       </c>
       <c r="F99" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G99" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I99" t="inlineStr"/>
     </row>
@@ -3167,13 +3167,13 @@
         <v>32</v>
       </c>
       <c r="C100" t="n">
-        <v>0.00049</v>
+        <v>0.13285</v>
       </c>
       <c r="D100" t="n">
-        <v>0.00049</v>
+        <v>0.13285</v>
       </c>
       <c r="E100" t="n">
-        <v>0.0005</v>
+        <v>0.13286</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -3194,7 +3194,7 @@
         <v>32</v>
       </c>
       <c r="C101" t="n">
-        <v>0.0005</v>
+        <v>0.13286</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
@@ -3212,7 +3212,7 @@
         <v>3</v>
       </c>
       <c r="I101" t="n">
-        <v>5e-05</v>
+        <v>2e-05</v>
       </c>
     </row>
     <row r="102">
@@ -3223,22 +3223,22 @@
         <v>33</v>
       </c>
       <c r="C102" t="n">
-        <v>0.00047</v>
+        <v>0.13723</v>
       </c>
       <c r="D102" t="n">
-        <v>0.00049</v>
+        <v>0.13723</v>
       </c>
       <c r="E102" t="n">
-        <v>0.0005</v>
+        <v>0.13723</v>
       </c>
       <c r="F102" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G102" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H102" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I102" t="inlineStr"/>
     </row>
@@ -3250,13 +3250,13 @@
         <v>33</v>
       </c>
       <c r="C103" t="n">
-        <v>0.0005</v>
+        <v>0.13723</v>
       </c>
       <c r="D103" t="n">
-        <v>0.0005</v>
+        <v>0.13723</v>
       </c>
       <c r="E103" t="n">
-        <v>0.00051</v>
+        <v>0.13724</v>
       </c>
       <c r="F103" t="n">
         <v>0</v>
@@ -3277,7 +3277,7 @@
         <v>33</v>
       </c>
       <c r="C104" t="n">
-        <v>0.00051</v>
+        <v>0.13724</v>
       </c>
       <c r="D104" t="n">
         <v>0</v>
@@ -3295,1501 +3295,7 @@
         <v>3</v>
       </c>
       <c r="I104" t="n">
-        <v>4e-05</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" s="1" t="n">
-        <v>102</v>
-      </c>
-      <c r="B105" t="n">
-        <v>34</v>
-      </c>
-      <c r="C105" t="n">
-        <v>0.00048</v>
-      </c>
-      <c r="D105" t="n">
-        <v>0.0005</v>
-      </c>
-      <c r="E105" t="n">
-        <v>0.00051</v>
-      </c>
-      <c r="F105" t="n">
-        <v>3</v>
-      </c>
-      <c r="G105" t="n">
-        <v>4</v>
-      </c>
-      <c r="H105" t="n">
-        <v>1</v>
-      </c>
-      <c r="I105" t="inlineStr"/>
-    </row>
-    <row r="106">
-      <c r="A106" s="1" t="n">
-        <v>103</v>
-      </c>
-      <c r="B106" t="n">
-        <v>34</v>
-      </c>
-      <c r="C106" t="n">
-        <v>0.00051</v>
-      </c>
-      <c r="D106" t="n">
-        <v>0.00051</v>
-      </c>
-      <c r="E106" t="n">
-        <v>0.00052</v>
-      </c>
-      <c r="F106" t="n">
-        <v>0</v>
-      </c>
-      <c r="G106" t="n">
-        <v>1</v>
-      </c>
-      <c r="H106" t="n">
-        <v>2</v>
-      </c>
-      <c r="I106" t="inlineStr"/>
-    </row>
-    <row r="107">
-      <c r="A107" s="1" t="n">
-        <v>104</v>
-      </c>
-      <c r="B107" t="n">
-        <v>34</v>
-      </c>
-      <c r="C107" t="n">
-        <v>0.00052</v>
-      </c>
-      <c r="D107" t="n">
-        <v>0</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0</v>
-      </c>
-      <c r="F107" t="n">
-        <v>0</v>
-      </c>
-      <c r="G107" t="n">
-        <v>0</v>
-      </c>
-      <c r="H107" t="n">
-        <v>3</v>
-      </c>
-      <c r="I107" t="n">
-        <v>5e-05</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="B108" t="n">
-        <v>35</v>
-      </c>
-      <c r="C108" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="D108" t="n">
-        <v>0.00054</v>
-      </c>
-      <c r="E108" t="n">
-        <v>0.00055</v>
-      </c>
-      <c r="F108" t="n">
-        <v>0</v>
-      </c>
-      <c r="G108" t="n">
-        <v>1</v>
-      </c>
-      <c r="H108" t="n">
-        <v>1</v>
-      </c>
-      <c r="I108" t="inlineStr"/>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="n">
-        <v>106</v>
-      </c>
-      <c r="B109" t="n">
-        <v>35</v>
-      </c>
-      <c r="C109" t="n">
-        <v>0.00055</v>
-      </c>
-      <c r="D109" t="n">
-        <v>0.00055</v>
-      </c>
-      <c r="E109" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="F109" t="n">
-        <v>0</v>
-      </c>
-      <c r="G109" t="n">
-        <v>1</v>
-      </c>
-      <c r="H109" t="n">
-        <v>2</v>
-      </c>
-      <c r="I109" t="inlineStr"/>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="n">
-        <v>107</v>
-      </c>
-      <c r="B110" t="n">
-        <v>35</v>
-      </c>
-      <c r="C110" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="D110" t="n">
-        <v>0</v>
-      </c>
-      <c r="E110" t="n">
-        <v>0</v>
-      </c>
-      <c r="F110" t="n">
-        <v>0</v>
-      </c>
-      <c r="G110" t="n">
-        <v>0</v>
-      </c>
-      <c r="H110" t="n">
-        <v>3</v>
-      </c>
-      <c r="I110" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>108</v>
-      </c>
-      <c r="B111" t="n">
-        <v>36</v>
-      </c>
-      <c r="C111" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="D111" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="E111" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="F111" t="n">
-        <v>0</v>
-      </c>
-      <c r="G111" t="n">
-        <v>1</v>
-      </c>
-      <c r="H111" t="n">
-        <v>1</v>
-      </c>
-      <c r="I111" t="inlineStr"/>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B112" t="n">
-        <v>36</v>
-      </c>
-      <c r="C112" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="D112" t="n">
-        <v>0.00056</v>
-      </c>
-      <c r="E112" t="n">
-        <v>0.00058</v>
-      </c>
-      <c r="F112" t="n">
-        <v>0</v>
-      </c>
-      <c r="G112" t="n">
-        <v>1</v>
-      </c>
-      <c r="H112" t="n">
-        <v>2</v>
-      </c>
-      <c r="I112" t="inlineStr"/>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="n">
-        <v>110</v>
-      </c>
-      <c r="B113" t="n">
-        <v>36</v>
-      </c>
-      <c r="C113" t="n">
-        <v>0.00058</v>
-      </c>
-      <c r="D113" t="n">
-        <v>0</v>
-      </c>
-      <c r="E113" t="n">
-        <v>0</v>
-      </c>
-      <c r="F113" t="n">
-        <v>0</v>
-      </c>
-      <c r="G113" t="n">
-        <v>0</v>
-      </c>
-      <c r="H113" t="n">
-        <v>3</v>
-      </c>
-      <c r="I113" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="n">
-        <v>111</v>
-      </c>
-      <c r="B114" t="n">
-        <v>37</v>
-      </c>
-      <c r="C114" t="n">
-        <v>0.00061</v>
-      </c>
-      <c r="D114" t="n">
-        <v>0.00061</v>
-      </c>
-      <c r="E114" t="n">
-        <v>0.00061</v>
-      </c>
-      <c r="F114" t="n">
-        <v>0</v>
-      </c>
-      <c r="G114" t="n">
-        <v>1</v>
-      </c>
-      <c r="H114" t="n">
-        <v>1</v>
-      </c>
-      <c r="I114" t="inlineStr"/>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="n">
-        <v>112</v>
-      </c>
-      <c r="B115" t="n">
-        <v>37</v>
-      </c>
-      <c r="C115" t="n">
-        <v>0.00061</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0.00061</v>
-      </c>
-      <c r="E115" t="n">
-        <v>0.00062</v>
-      </c>
-      <c r="F115" t="n">
-        <v>0</v>
-      </c>
-      <c r="G115" t="n">
-        <v>1</v>
-      </c>
-      <c r="H115" t="n">
-        <v>2</v>
-      </c>
-      <c r="I115" t="inlineStr"/>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="n">
-        <v>113</v>
-      </c>
-      <c r="B116" t="n">
-        <v>37</v>
-      </c>
-      <c r="C116" t="n">
-        <v>0.00062</v>
-      </c>
-      <c r="D116" t="n">
-        <v>0</v>
-      </c>
-      <c r="E116" t="n">
-        <v>0</v>
-      </c>
-      <c r="F116" t="n">
-        <v>0</v>
-      </c>
-      <c r="G116" t="n">
-        <v>0</v>
-      </c>
-      <c r="H116" t="n">
-        <v>3</v>
-      </c>
-      <c r="I116" t="n">
         <v>1e-05</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="n">
-        <v>114</v>
-      </c>
-      <c r="B117" t="n">
-        <v>38</v>
-      </c>
-      <c r="C117" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="D117" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="E117" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="F117" t="n">
-        <v>0</v>
-      </c>
-      <c r="G117" t="n">
-        <v>1</v>
-      </c>
-      <c r="H117" t="n">
-        <v>1</v>
-      </c>
-      <c r="I117" t="inlineStr"/>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="n">
-        <v>115</v>
-      </c>
-      <c r="B118" t="n">
-        <v>38</v>
-      </c>
-      <c r="C118" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="D118" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="E118" t="n">
-        <v>0.0006400000000000001</v>
-      </c>
-      <c r="F118" t="n">
-        <v>0</v>
-      </c>
-      <c r="G118" t="n">
-        <v>1</v>
-      </c>
-      <c r="H118" t="n">
-        <v>2</v>
-      </c>
-      <c r="I118" t="inlineStr"/>
-    </row>
-    <row r="119">
-      <c r="A119" s="1" t="n">
-        <v>116</v>
-      </c>
-      <c r="B119" t="n">
-        <v>38</v>
-      </c>
-      <c r="C119" t="n">
-        <v>0.0006400000000000001</v>
-      </c>
-      <c r="D119" t="n">
-        <v>0</v>
-      </c>
-      <c r="E119" t="n">
-        <v>0</v>
-      </c>
-      <c r="F119" t="n">
-        <v>0</v>
-      </c>
-      <c r="G119" t="n">
-        <v>0</v>
-      </c>
-      <c r="H119" t="n">
-        <v>3</v>
-      </c>
-      <c r="I119" t="n">
-        <v>1e-05</v>
-      </c>
-    </row>
-    <row r="120">
-      <c r="A120" s="1" t="n">
-        <v>117</v>
-      </c>
-      <c r="B120" t="n">
-        <v>39</v>
-      </c>
-      <c r="C120" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="D120" t="n">
-        <v>0.00063</v>
-      </c>
-      <c r="E120" t="n">
-        <v>0.0006400000000000001</v>
-      </c>
-      <c r="F120" t="n">
-        <v>0</v>
-      </c>
-      <c r="G120" t="n">
-        <v>1</v>
-      </c>
-      <c r="H120" t="n">
-        <v>1</v>
-      </c>
-      <c r="I120" t="inlineStr"/>
-    </row>
-    <row r="121">
-      <c r="A121" s="1" t="n">
-        <v>118</v>
-      </c>
-      <c r="B121" t="n">
-        <v>39</v>
-      </c>
-      <c r="C121" t="n">
-        <v>0.0006400000000000001</v>
-      </c>
-      <c r="D121" t="n">
-        <v>0.0006400000000000001</v>
-      </c>
-      <c r="E121" t="n">
-        <v>0.00065</v>
-      </c>
-      <c r="F121" t="n">
-        <v>0</v>
-      </c>
-      <c r="G121" t="n">
-        <v>1</v>
-      </c>
-      <c r="H121" t="n">
-        <v>2</v>
-      </c>
-      <c r="I121" t="inlineStr"/>
-    </row>
-    <row r="122">
-      <c r="A122" s="1" t="n">
-        <v>119</v>
-      </c>
-      <c r="B122" t="n">
-        <v>39</v>
-      </c>
-      <c r="C122" t="n">
-        <v>0.00065</v>
-      </c>
-      <c r="D122" t="n">
-        <v>0</v>
-      </c>
-      <c r="E122" t="n">
-        <v>0</v>
-      </c>
-      <c r="F122" t="n">
-        <v>0</v>
-      </c>
-      <c r="G122" t="n">
-        <v>0</v>
-      </c>
-      <c r="H122" t="n">
-        <v>3</v>
-      </c>
-      <c r="I122" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" s="1" t="n">
-        <v>120</v>
-      </c>
-      <c r="B123" t="n">
-        <v>40</v>
-      </c>
-      <c r="C123" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="D123" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="E123" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="F123" t="n">
-        <v>0</v>
-      </c>
-      <c r="G123" t="n">
-        <v>1</v>
-      </c>
-      <c r="H123" t="n">
-        <v>1</v>
-      </c>
-      <c r="I123" t="inlineStr"/>
-    </row>
-    <row r="124">
-      <c r="A124" s="1" t="n">
-        <v>121</v>
-      </c>
-      <c r="B124" t="n">
-        <v>40</v>
-      </c>
-      <c r="C124" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="D124" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="E124" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="F124" t="n">
-        <v>0</v>
-      </c>
-      <c r="G124" t="n">
-        <v>1</v>
-      </c>
-      <c r="H124" t="n">
-        <v>2</v>
-      </c>
-      <c r="I124" t="inlineStr"/>
-    </row>
-    <row r="125">
-      <c r="A125" s="1" t="n">
-        <v>122</v>
-      </c>
-      <c r="B125" t="n">
-        <v>40</v>
-      </c>
-      <c r="C125" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="D125" t="n">
-        <v>0</v>
-      </c>
-      <c r="E125" t="n">
-        <v>0</v>
-      </c>
-      <c r="F125" t="n">
-        <v>0</v>
-      </c>
-      <c r="G125" t="n">
-        <v>0</v>
-      </c>
-      <c r="H125" t="n">
-        <v>3</v>
-      </c>
-      <c r="I125" t="n">
-        <v>1e-05</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" s="1" t="n">
-        <v>123</v>
-      </c>
-      <c r="B126" t="n">
-        <v>41</v>
-      </c>
-      <c r="C126" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="D126" t="n">
-        <v>0.00066</v>
-      </c>
-      <c r="E126" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="F126" t="n">
-        <v>0</v>
-      </c>
-      <c r="G126" t="n">
-        <v>1</v>
-      </c>
-      <c r="H126" t="n">
-        <v>1</v>
-      </c>
-      <c r="I126" t="inlineStr"/>
-    </row>
-    <row r="127">
-      <c r="A127" s="1" t="n">
-        <v>124</v>
-      </c>
-      <c r="B127" t="n">
-        <v>41</v>
-      </c>
-      <c r="C127" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="D127" t="n">
-        <v>0.00067</v>
-      </c>
-      <c r="E127" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="F127" t="n">
-        <v>0</v>
-      </c>
-      <c r="G127" t="n">
-        <v>1</v>
-      </c>
-      <c r="H127" t="n">
-        <v>2</v>
-      </c>
-      <c r="I127" t="inlineStr"/>
-    </row>
-    <row r="128">
-      <c r="A128" s="1" t="n">
-        <v>125</v>
-      </c>
-      <c r="B128" t="n">
-        <v>41</v>
-      </c>
-      <c r="C128" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="D128" t="n">
-        <v>0</v>
-      </c>
-      <c r="E128" t="n">
-        <v>0</v>
-      </c>
-      <c r="F128" t="n">
-        <v>0</v>
-      </c>
-      <c r="G128" t="n">
-        <v>0</v>
-      </c>
-      <c r="H128" t="n">
-        <v>3</v>
-      </c>
-      <c r="I128" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" s="1" t="n">
-        <v>126</v>
-      </c>
-      <c r="B129" t="n">
-        <v>42</v>
-      </c>
-      <c r="C129" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="D129" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="E129" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="F129" t="n">
-        <v>0</v>
-      </c>
-      <c r="G129" t="n">
-        <v>1</v>
-      </c>
-      <c r="H129" t="n">
-        <v>1</v>
-      </c>
-      <c r="I129" t="inlineStr"/>
-    </row>
-    <row r="130">
-      <c r="A130" s="1" t="n">
-        <v>127</v>
-      </c>
-      <c r="B130" t="n">
-        <v>42</v>
-      </c>
-      <c r="C130" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="D130" t="n">
-        <v>0.00068</v>
-      </c>
-      <c r="E130" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="F130" t="n">
-        <v>0</v>
-      </c>
-      <c r="G130" t="n">
-        <v>1</v>
-      </c>
-      <c r="H130" t="n">
-        <v>2</v>
-      </c>
-      <c r="I130" t="inlineStr"/>
-    </row>
-    <row r="131">
-      <c r="A131" s="1" t="n">
-        <v>128</v>
-      </c>
-      <c r="B131" t="n">
-        <v>42</v>
-      </c>
-      <c r="C131" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="D131" t="n">
-        <v>0</v>
-      </c>
-      <c r="E131" t="n">
-        <v>0</v>
-      </c>
-      <c r="F131" t="n">
-        <v>0</v>
-      </c>
-      <c r="G131" t="n">
-        <v>0</v>
-      </c>
-      <c r="H131" t="n">
-        <v>3</v>
-      </c>
-      <c r="I131" t="n">
-        <v>1e-05</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" s="1" t="n">
-        <v>129</v>
-      </c>
-      <c r="B132" t="n">
-        <v>43</v>
-      </c>
-      <c r="C132" t="n">
-        <v>0.00069</v>
-      </c>
-      <c r="D132" t="n">
-        <v>0.00069</v>
-      </c>
-      <c r="E132" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="F132" t="n">
-        <v>0</v>
-      </c>
-      <c r="G132" t="n">
-        <v>1</v>
-      </c>
-      <c r="H132" t="n">
-        <v>1</v>
-      </c>
-      <c r="I132" t="inlineStr"/>
-    </row>
-    <row r="133">
-      <c r="A133" s="1" t="n">
-        <v>130</v>
-      </c>
-      <c r="B133" t="n">
-        <v>43</v>
-      </c>
-      <c r="C133" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="D133" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="E133" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="F133" t="n">
-        <v>0</v>
-      </c>
-      <c r="G133" t="n">
-        <v>1</v>
-      </c>
-      <c r="H133" t="n">
-        <v>2</v>
-      </c>
-      <c r="I133" t="inlineStr"/>
-    </row>
-    <row r="134">
-      <c r="A134" s="1" t="n">
-        <v>131</v>
-      </c>
-      <c r="B134" t="n">
-        <v>43</v>
-      </c>
-      <c r="C134" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="D134" t="n">
-        <v>0</v>
-      </c>
-      <c r="E134" t="n">
-        <v>0</v>
-      </c>
-      <c r="F134" t="n">
-        <v>0</v>
-      </c>
-      <c r="G134" t="n">
-        <v>0</v>
-      </c>
-      <c r="H134" t="n">
-        <v>3</v>
-      </c>
-      <c r="I134" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" s="1" t="n">
-        <v>132</v>
-      </c>
-      <c r="B135" t="n">
-        <v>44</v>
-      </c>
-      <c r="C135" t="n">
-        <v>0.00069</v>
-      </c>
-      <c r="D135" t="n">
-        <v>0.0007</v>
-      </c>
-      <c r="E135" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="F135" t="n">
-        <v>1</v>
-      </c>
-      <c r="G135" t="n">
-        <v>2</v>
-      </c>
-      <c r="H135" t="n">
-        <v>1</v>
-      </c>
-      <c r="I135" t="inlineStr"/>
-    </row>
-    <row r="136">
-      <c r="A136" s="1" t="n">
-        <v>133</v>
-      </c>
-      <c r="B136" t="n">
-        <v>44</v>
-      </c>
-      <c r="C136" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="D136" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="E136" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="F136" t="n">
-        <v>0</v>
-      </c>
-      <c r="G136" t="n">
-        <v>1</v>
-      </c>
-      <c r="H136" t="n">
-        <v>2</v>
-      </c>
-      <c r="I136" t="inlineStr"/>
-    </row>
-    <row r="137">
-      <c r="A137" s="1" t="n">
-        <v>134</v>
-      </c>
-      <c r="B137" t="n">
-        <v>44</v>
-      </c>
-      <c r="C137" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="D137" t="n">
-        <v>0</v>
-      </c>
-      <c r="E137" t="n">
-        <v>0</v>
-      </c>
-      <c r="F137" t="n">
-        <v>0</v>
-      </c>
-      <c r="G137" t="n">
-        <v>0</v>
-      </c>
-      <c r="H137" t="n">
-        <v>3</v>
-      </c>
-      <c r="I137" t="n">
-        <v>3e-05</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" s="1" t="n">
-        <v>135</v>
-      </c>
-      <c r="B138" t="n">
-        <v>45</v>
-      </c>
-      <c r="C138" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="D138" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="E138" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="F138" t="n">
-        <v>1</v>
-      </c>
-      <c r="G138" t="n">
-        <v>2</v>
-      </c>
-      <c r="H138" t="n">
-        <v>1</v>
-      </c>
-      <c r="I138" t="inlineStr"/>
-    </row>
-    <row r="139">
-      <c r="A139" s="1" t="n">
-        <v>136</v>
-      </c>
-      <c r="B139" t="n">
-        <v>45</v>
-      </c>
-      <c r="C139" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="D139" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="E139" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="F139" t="n">
-        <v>0</v>
-      </c>
-      <c r="G139" t="n">
-        <v>1</v>
-      </c>
-      <c r="H139" t="n">
-        <v>2</v>
-      </c>
-      <c r="I139" t="inlineStr"/>
-    </row>
-    <row r="140">
-      <c r="A140" s="1" t="n">
-        <v>137</v>
-      </c>
-      <c r="B140" t="n">
-        <v>45</v>
-      </c>
-      <c r="C140" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="D140" t="n">
-        <v>0</v>
-      </c>
-      <c r="E140" t="n">
-        <v>0</v>
-      </c>
-      <c r="F140" t="n">
-        <v>0</v>
-      </c>
-      <c r="G140" t="n">
-        <v>0</v>
-      </c>
-      <c r="H140" t="n">
-        <v>3</v>
-      </c>
-      <c r="I140" t="n">
-        <v>3e-05</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" s="1" t="n">
-        <v>138</v>
-      </c>
-      <c r="B141" t="n">
-        <v>46</v>
-      </c>
-      <c r="C141" t="n">
-        <v>0.00071</v>
-      </c>
-      <c r="D141" t="n">
-        <v>0.00072</v>
-      </c>
-      <c r="E141" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="F141" t="n">
-        <v>2</v>
-      </c>
-      <c r="G141" t="n">
-        <v>3</v>
-      </c>
-      <c r="H141" t="n">
-        <v>1</v>
-      </c>
-      <c r="I141" t="inlineStr"/>
-    </row>
-    <row r="142">
-      <c r="A142" s="1" t="n">
-        <v>139</v>
-      </c>
-      <c r="B142" t="n">
-        <v>46</v>
-      </c>
-      <c r="C142" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="D142" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="E142" t="n">
-        <v>0.00074</v>
-      </c>
-      <c r="F142" t="n">
-        <v>0</v>
-      </c>
-      <c r="G142" t="n">
-        <v>1</v>
-      </c>
-      <c r="H142" t="n">
-        <v>2</v>
-      </c>
-      <c r="I142" t="inlineStr"/>
-    </row>
-    <row r="143">
-      <c r="A143" s="1" t="n">
-        <v>140</v>
-      </c>
-      <c r="B143" t="n">
-        <v>46</v>
-      </c>
-      <c r="C143" t="n">
-        <v>0.00074</v>
-      </c>
-      <c r="D143" t="n">
-        <v>0</v>
-      </c>
-      <c r="E143" t="n">
-        <v>0</v>
-      </c>
-      <c r="F143" t="n">
-        <v>0</v>
-      </c>
-      <c r="G143" t="n">
-        <v>0</v>
-      </c>
-      <c r="H143" t="n">
-        <v>3</v>
-      </c>
-      <c r="I143" t="n">
-        <v>4e-05</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" s="1" t="n">
-        <v>141</v>
-      </c>
-      <c r="B144" t="n">
-        <v>47</v>
-      </c>
-      <c r="C144" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="D144" t="n">
-        <v>0.00073</v>
-      </c>
-      <c r="E144" t="n">
-        <v>0.00074</v>
-      </c>
-      <c r="F144" t="n">
-        <v>0</v>
-      </c>
-      <c r="G144" t="n">
-        <v>1</v>
-      </c>
-      <c r="H144" t="n">
-        <v>1</v>
-      </c>
-      <c r="I144" t="inlineStr"/>
-    </row>
-    <row r="145">
-      <c r="A145" s="1" t="n">
-        <v>142</v>
-      </c>
-      <c r="B145" t="n">
-        <v>47</v>
-      </c>
-      <c r="C145" t="n">
-        <v>0.00074</v>
-      </c>
-      <c r="D145" t="n">
-        <v>0.00074</v>
-      </c>
-      <c r="E145" t="n">
-        <v>0.00076</v>
-      </c>
-      <c r="F145" t="n">
-        <v>0</v>
-      </c>
-      <c r="G145" t="n">
-        <v>1</v>
-      </c>
-      <c r="H145" t="n">
-        <v>2</v>
-      </c>
-      <c r="I145" t="inlineStr"/>
-    </row>
-    <row r="146">
-      <c r="A146" s="1" t="n">
-        <v>143</v>
-      </c>
-      <c r="B146" t="n">
-        <v>47</v>
-      </c>
-      <c r="C146" t="n">
-        <v>0.00076</v>
-      </c>
-      <c r="D146" t="n">
-        <v>0</v>
-      </c>
-      <c r="E146" t="n">
-        <v>0</v>
-      </c>
-      <c r="F146" t="n">
-        <v>0</v>
-      </c>
-      <c r="G146" t="n">
-        <v>0</v>
-      </c>
-      <c r="H146" t="n">
-        <v>3</v>
-      </c>
-      <c r="I146" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" s="1" t="n">
-        <v>144</v>
-      </c>
-      <c r="B147" t="n">
-        <v>48</v>
-      </c>
-      <c r="C147" t="n">
-        <v>0.00076</v>
-      </c>
-      <c r="D147" t="n">
-        <v>0.00076</v>
-      </c>
-      <c r="E147" t="n">
-        <v>0.00077</v>
-      </c>
-      <c r="F147" t="n">
-        <v>0</v>
-      </c>
-      <c r="G147" t="n">
-        <v>1</v>
-      </c>
-      <c r="H147" t="n">
-        <v>1</v>
-      </c>
-      <c r="I147" t="inlineStr"/>
-    </row>
-    <row r="148">
-      <c r="A148" s="1" t="n">
-        <v>145</v>
-      </c>
-      <c r="B148" t="n">
-        <v>48</v>
-      </c>
-      <c r="C148" t="n">
-        <v>0.00077</v>
-      </c>
-      <c r="D148" t="n">
-        <v>0.00077</v>
-      </c>
-      <c r="E148" t="n">
-        <v>0.00078</v>
-      </c>
-      <c r="F148" t="n">
-        <v>0</v>
-      </c>
-      <c r="G148" t="n">
-        <v>1</v>
-      </c>
-      <c r="H148" t="n">
-        <v>2</v>
-      </c>
-      <c r="I148" t="inlineStr"/>
-    </row>
-    <row r="149">
-      <c r="A149" s="1" t="n">
-        <v>146</v>
-      </c>
-      <c r="B149" t="n">
-        <v>48</v>
-      </c>
-      <c r="C149" t="n">
-        <v>0.00078</v>
-      </c>
-      <c r="D149" t="n">
-        <v>0</v>
-      </c>
-      <c r="E149" t="n">
-        <v>0</v>
-      </c>
-      <c r="F149" t="n">
-        <v>0</v>
-      </c>
-      <c r="G149" t="n">
-        <v>0</v>
-      </c>
-      <c r="H149" t="n">
-        <v>3</v>
-      </c>
-      <c r="I149" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" s="1" t="n">
-        <v>147</v>
-      </c>
-      <c r="B150" t="n">
-        <v>49</v>
-      </c>
-      <c r="C150" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="D150" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="E150" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="F150" t="n">
-        <v>0</v>
-      </c>
-      <c r="G150" t="n">
-        <v>1</v>
-      </c>
-      <c r="H150" t="n">
-        <v>1</v>
-      </c>
-      <c r="I150" t="inlineStr"/>
-    </row>
-    <row r="151">
-      <c r="A151" s="1" t="n">
-        <v>148</v>
-      </c>
-      <c r="B151" t="n">
-        <v>49</v>
-      </c>
-      <c r="C151" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="D151" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="E151" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="F151" t="n">
-        <v>0</v>
-      </c>
-      <c r="G151" t="n">
-        <v>1</v>
-      </c>
-      <c r="H151" t="n">
-        <v>2</v>
-      </c>
-      <c r="I151" t="inlineStr"/>
-    </row>
-    <row r="152">
-      <c r="A152" s="1" t="n">
-        <v>149</v>
-      </c>
-      <c r="B152" t="n">
-        <v>49</v>
-      </c>
-      <c r="C152" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="D152" t="n">
-        <v>0</v>
-      </c>
-      <c r="E152" t="n">
-        <v>0</v>
-      </c>
-      <c r="F152" t="n">
-        <v>0</v>
-      </c>
-      <c r="G152" t="n">
-        <v>0</v>
-      </c>
-      <c r="H152" t="n">
-        <v>3</v>
-      </c>
-      <c r="I152" t="n">
-        <v>1e-05</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" s="1" t="n">
-        <v>150</v>
-      </c>
-      <c r="B153" t="n">
-        <v>50</v>
-      </c>
-      <c r="C153" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="D153" t="n">
-        <v>0.00079</v>
-      </c>
-      <c r="E153" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="F153" t="n">
-        <v>0</v>
-      </c>
-      <c r="G153" t="n">
-        <v>1</v>
-      </c>
-      <c r="H153" t="n">
-        <v>1</v>
-      </c>
-      <c r="I153" t="inlineStr"/>
-    </row>
-    <row r="154">
-      <c r="A154" s="1" t="n">
-        <v>151</v>
-      </c>
-      <c r="B154" t="n">
-        <v>50</v>
-      </c>
-      <c r="C154" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="D154" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="E154" t="n">
-        <v>0.00081</v>
-      </c>
-      <c r="F154" t="n">
-        <v>0</v>
-      </c>
-      <c r="G154" t="n">
-        <v>1</v>
-      </c>
-      <c r="H154" t="n">
-        <v>2</v>
-      </c>
-      <c r="I154" t="inlineStr"/>
-    </row>
-    <row r="155">
-      <c r="A155" s="1" t="n">
-        <v>152</v>
-      </c>
-      <c r="B155" t="n">
-        <v>50</v>
-      </c>
-      <c r="C155" t="n">
-        <v>0.00081</v>
-      </c>
-      <c r="D155" t="n">
-        <v>0</v>
-      </c>
-      <c r="E155" t="n">
-        <v>0</v>
-      </c>
-      <c r="F155" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" t="n">
-        <v>0</v>
-      </c>
-      <c r="H155" t="n">
-        <v>3</v>
-      </c>
-      <c r="I155" t="n">
-        <v>2e-05</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" s="1" t="n">
-        <v>153</v>
-      </c>
-      <c r="B156" t="n">
-        <v>51</v>
-      </c>
-      <c r="C156" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="D156" t="n">
-        <v>0.0008</v>
-      </c>
-      <c r="E156" t="n">
-        <v>0.00081</v>
-      </c>
-      <c r="F156" t="n">
-        <v>0</v>
-      </c>
-      <c r="G156" t="n">
-        <v>1</v>
-      </c>
-      <c r="H156" t="n">
-        <v>1</v>
-      </c>
-      <c r="I156" t="inlineStr"/>
-    </row>
-    <row r="157">
-      <c r="A157" s="1" t="n">
-        <v>154</v>
-      </c>
-      <c r="B157" t="n">
-        <v>51</v>
-      </c>
-      <c r="C157" t="n">
-        <v>0.00081</v>
-      </c>
-      <c r="D157" t="n">
-        <v>0.00081</v>
-      </c>
-      <c r="E157" t="n">
-        <v>0.00082</v>
-      </c>
-      <c r="F157" t="n">
-        <v>0</v>
-      </c>
-      <c r="G157" t="n">
-        <v>1</v>
-      </c>
-      <c r="H157" t="n">
-        <v>2</v>
-      </c>
-      <c r="I157" t="inlineStr"/>
-    </row>
-    <row r="158">
-      <c r="A158" s="1" t="n">
-        <v>155</v>
-      </c>
-      <c r="B158" t="n">
-        <v>51</v>
-      </c>
-      <c r="C158" t="n">
-        <v>0.00082</v>
-      </c>
-      <c r="D158" t="n">
-        <v>0</v>
-      </c>
-      <c r="E158" t="n">
-        <v>0</v>
-      </c>
-      <c r="F158" t="n">
-        <v>0</v>
-      </c>
-      <c r="G158" t="n">
-        <v>0</v>
-      </c>
-      <c r="H158" t="n">
-        <v>3</v>
-      </c>
-      <c r="I158" t="n">
-        <v>2e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>